<commit_message>
Last commit, a lot of things changed
</commit_message>
<xml_diff>
--- a/Lab2_Uzduotys (1).xlsx
+++ b/Lab2_Uzduotys (1).xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21328"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matas\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Universitetas\ANTRAS-KURSAS\Duomenu-Struktura\Duomenu-Strukturos-Lab2\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDD63864-9B06-4EA6-8F95-DDDD1D022E51}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19905" windowHeight="8715" activeTab="1"/>
+    <workbookView xWindow="-19320" yWindow="600" windowWidth="19440" windowHeight="15000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Studentai" sheetId="7" r:id="rId1"/>
@@ -1235,7 +1236,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="11">
     <font>
       <sz val="11"/>
@@ -1329,7 +1330,7 @@
       <name val="Arial Unicode MS"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1348,6 +1349,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -1362,7 +1369,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1399,23 +1406,39 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1511,6 +1534,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -1546,6 +1586,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1721,12 +1778,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P354"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M22" sqref="M22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A289" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="M304" sqref="M304"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -10173,7 +10230,7 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="J5" r:id="rId1"/>
+    <hyperlink ref="J5" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId2"/>
@@ -10181,12 +10238,12 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D43"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C25" sqref="C25"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -10199,7 +10256,7 @@
     <col min="7" max="7" width="21.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="1" customFormat="1" ht="25.9">
+    <row r="1" spans="1:3" s="1" customFormat="1" ht="26.25">
       <c r="A1" s="11" t="s">
         <v>3</v>
       </c>
@@ -10211,28 +10268,28 @@
       </c>
     </row>
     <row r="2" spans="1:3">
-      <c r="A2" s="21">
-        <v>1</v>
-      </c>
-      <c r="B2" s="18" t="s">
+      <c r="A2" s="29">
+        <v>1</v>
+      </c>
+      <c r="B2" s="26" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="8" t="s">
+      <c r="C2" s="20" t="s">
         <v>394</v>
       </c>
     </row>
     <row r="3" spans="1:3">
-      <c r="A3" s="21"/>
-      <c r="B3" s="18"/>
-      <c r="C3" s="9" t="s">
+      <c r="A3" s="29"/>
+      <c r="B3" s="26"/>
+      <c r="C3" s="21" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:3">
-      <c r="A4" s="21">
-        <v>2</v>
-      </c>
-      <c r="B4" s="18" t="s">
+      <c r="A4" s="27">
+        <v>2</v>
+      </c>
+      <c r="B4" s="23" t="s">
         <v>0</v>
       </c>
       <c r="C4" s="8" t="s">
@@ -10240,17 +10297,17 @@
       </c>
     </row>
     <row r="5" spans="1:3" ht="15" customHeight="1">
-      <c r="A5" s="21"/>
-      <c r="B5" s="18"/>
+      <c r="A5" s="27"/>
+      <c r="B5" s="23"/>
       <c r="C5" s="9" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="6" spans="1:3">
-      <c r="A6" s="21">
-        <v>3</v>
-      </c>
-      <c r="B6" s="18" t="s">
+      <c r="A6" s="27">
+        <v>3</v>
+      </c>
+      <c r="B6" s="23" t="s">
         <v>0</v>
       </c>
       <c r="C6" s="8" t="s">
@@ -10258,35 +10315,35 @@
       </c>
     </row>
     <row r="7" spans="1:3">
-      <c r="A7" s="21"/>
-      <c r="B7" s="18"/>
+      <c r="A7" s="27"/>
+      <c r="B7" s="23"/>
       <c r="C7" s="9" t="s">
         <v>399</v>
       </c>
     </row>
     <row r="8" spans="1:3">
-      <c r="A8" s="21">
-        <v>4</v>
-      </c>
-      <c r="B8" s="18" t="s">
+      <c r="A8" s="29">
+        <v>4</v>
+      </c>
+      <c r="B8" s="26" t="s">
         <v>0</v>
       </c>
-      <c r="C8" s="8" t="s">
+      <c r="C8" s="20" t="s">
         <v>397</v>
       </c>
     </row>
     <row r="9" spans="1:3">
-      <c r="A9" s="21"/>
-      <c r="B9" s="18"/>
-      <c r="C9" s="9" t="s">
+      <c r="A9" s="29"/>
+      <c r="B9" s="26"/>
+      <c r="C9" s="21" t="s">
         <v>400</v>
       </c>
     </row>
     <row r="10" spans="1:3">
-      <c r="A10" s="21">
+      <c r="A10" s="27">
         <v>5</v>
       </c>
-      <c r="B10" s="19" t="s">
+      <c r="B10" s="24" t="s">
         <v>1</v>
       </c>
       <c r="C10" s="8" t="s">
@@ -10294,17 +10351,17 @@
       </c>
     </row>
     <row r="11" spans="1:3">
-      <c r="A11" s="21"/>
-      <c r="B11" s="19"/>
+      <c r="A11" s="27"/>
+      <c r="B11" s="24"/>
       <c r="C11" s="9" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="12" spans="1:3">
-      <c r="A12" s="21">
+      <c r="A12" s="27">
         <v>6</v>
       </c>
-      <c r="B12" s="19" t="s">
+      <c r="B12" s="24" t="s">
         <v>1</v>
       </c>
       <c r="C12" s="8" t="s">
@@ -10312,17 +10369,17 @@
       </c>
     </row>
     <row r="13" spans="1:3">
-      <c r="A13" s="21"/>
-      <c r="B13" s="19"/>
+      <c r="A13" s="27"/>
+      <c r="B13" s="24"/>
       <c r="C13" s="9" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="14" spans="1:3">
-      <c r="A14" s="21">
+      <c r="A14" s="27">
         <v>7</v>
       </c>
-      <c r="B14" s="18" t="s">
+      <c r="B14" s="23" t="s">
         <v>398</v>
       </c>
       <c r="C14" s="8" t="s">
@@ -10330,53 +10387,53 @@
       </c>
     </row>
     <row r="15" spans="1:3">
-      <c r="A15" s="21"/>
-      <c r="B15" s="18"/>
+      <c r="A15" s="27"/>
+      <c r="B15" s="23"/>
       <c r="C15" s="9" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="16" spans="1:3">
-      <c r="A16" s="21">
+      <c r="A16" s="29">
         <v>8</v>
       </c>
-      <c r="B16" s="18" t="s">
+      <c r="B16" s="26" t="s">
         <v>398</v>
       </c>
-      <c r="C16" s="8" t="s">
+      <c r="C16" s="20" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="17" spans="1:3">
-      <c r="A17" s="21"/>
-      <c r="B17" s="18"/>
-      <c r="C17" s="9" t="s">
+      <c r="A17" s="29"/>
+      <c r="B17" s="26"/>
+      <c r="C17" s="21" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="18" spans="1:3">
-      <c r="A18" s="21">
+      <c r="A18" s="29">
         <v>9</v>
       </c>
-      <c r="B18" s="19" t="s">
-        <v>1</v>
-      </c>
-      <c r="C18" s="8" t="s">
+      <c r="B18" s="25" t="s">
+        <v>1</v>
+      </c>
+      <c r="C18" s="20" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="19" spans="1:3">
-      <c r="A19" s="21"/>
-      <c r="B19" s="19"/>
-      <c r="C19" s="9" t="s">
+      <c r="A19" s="29"/>
+      <c r="B19" s="25"/>
+      <c r="C19" s="21" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="20" spans="1:3">
-      <c r="A20" s="21">
+      <c r="A20" s="27">
         <v>10</v>
       </c>
-      <c r="B20" s="19" t="s">
+      <c r="B20" s="24" t="s">
         <v>1</v>
       </c>
       <c r="C20" s="10" t="s">
@@ -10384,35 +10441,35 @@
       </c>
     </row>
     <row r="21" spans="1:3">
-      <c r="A21" s="21"/>
-      <c r="B21" s="19"/>
+      <c r="A21" s="27"/>
+      <c r="B21" s="24"/>
       <c r="C21" s="9" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="22" spans="1:3">
-      <c r="A22" s="21">
-        <v>11</v>
-      </c>
-      <c r="B22" s="19" t="s">
-        <v>1</v>
-      </c>
-      <c r="C22" s="8" t="s">
+      <c r="A22" s="29">
+        <v>11</v>
+      </c>
+      <c r="B22" s="25" t="s">
+        <v>1</v>
+      </c>
+      <c r="C22" s="20" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="23" spans="1:3">
-      <c r="A23" s="21"/>
-      <c r="B23" s="19"/>
-      <c r="C23" s="9" t="s">
+      <c r="A23" s="29"/>
+      <c r="B23" s="25"/>
+      <c r="C23" s="21" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="24" spans="1:3">
-      <c r="A24" s="21">
+      <c r="A24" s="27">
         <v>12</v>
       </c>
-      <c r="B24" s="19" t="s">
+      <c r="B24" s="24" t="s">
         <v>1</v>
       </c>
       <c r="C24" s="10" t="s">
@@ -10420,35 +10477,35 @@
       </c>
     </row>
     <row r="25" spans="1:3">
-      <c r="A25" s="21"/>
-      <c r="B25" s="19"/>
+      <c r="A25" s="27"/>
+      <c r="B25" s="24"/>
       <c r="C25" s="9" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="26" spans="1:3">
-      <c r="A26" s="21">
+      <c r="A26" s="29">
         <v>13</v>
       </c>
-      <c r="B26" s="19" t="s">
-        <v>1</v>
-      </c>
-      <c r="C26" s="10" t="s">
+      <c r="B26" s="25" t="s">
+        <v>1</v>
+      </c>
+      <c r="C26" s="22" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="27" spans="1:3">
-      <c r="A27" s="21"/>
-      <c r="B27" s="19"/>
-      <c r="C27" s="9" t="s">
+      <c r="A27" s="29"/>
+      <c r="B27" s="25"/>
+      <c r="C27" s="21" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="28" spans="1:3" ht="15" customHeight="1">
-      <c r="A28" s="21">
-        <v>14</v>
-      </c>
-      <c r="B28" s="18" t="s">
+      <c r="A28" s="27">
+        <v>14</v>
+      </c>
+      <c r="B28" s="23" t="s">
         <v>398</v>
       </c>
       <c r="C28" s="8" t="s">
@@ -10456,17 +10513,17 @@
       </c>
     </row>
     <row r="29" spans="1:3" ht="15" customHeight="1">
-      <c r="A29" s="21"/>
-      <c r="B29" s="18"/>
+      <c r="A29" s="27"/>
+      <c r="B29" s="23"/>
       <c r="C29" s="9" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="30" spans="1:3">
-      <c r="A30" s="21">
+      <c r="A30" s="27">
         <v>15</v>
       </c>
-      <c r="B30" s="18" t="s">
+      <c r="B30" s="23" t="s">
         <v>398</v>
       </c>
       <c r="C30" s="8" t="s">
@@ -10474,17 +10531,17 @@
       </c>
     </row>
     <row r="31" spans="1:3">
-      <c r="A31" s="21"/>
-      <c r="B31" s="18"/>
+      <c r="A31" s="27"/>
+      <c r="B31" s="23"/>
       <c r="C31" s="9" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="32" spans="1:3">
-      <c r="A32" s="21">
+      <c r="A32" s="27">
         <v>16</v>
       </c>
-      <c r="B32" s="18" t="s">
+      <c r="B32" s="23" t="s">
         <v>398</v>
       </c>
       <c r="C32" s="8" t="s">
@@ -10492,17 +10549,17 @@
       </c>
     </row>
     <row r="33" spans="1:4">
-      <c r="A33" s="21"/>
-      <c r="B33" s="18"/>
+      <c r="A33" s="27"/>
+      <c r="B33" s="23"/>
       <c r="C33" s="9" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="34" spans="1:4" ht="15" customHeight="1">
-      <c r="A34" s="21">
+      <c r="A34" s="27">
         <v>17</v>
       </c>
-      <c r="B34" s="18" t="s">
+      <c r="B34" s="23" t="s">
         <v>398</v>
       </c>
       <c r="C34" s="8" t="s">
@@ -10510,17 +10567,17 @@
       </c>
     </row>
     <row r="35" spans="1:4" ht="15" customHeight="1">
-      <c r="A35" s="21"/>
-      <c r="B35" s="18"/>
+      <c r="A35" s="27"/>
+      <c r="B35" s="23"/>
       <c r="C35" s="9" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="36" spans="1:4" ht="15" customHeight="1">
-      <c r="A36" s="21">
+      <c r="A36" s="27">
         <v>18</v>
       </c>
-      <c r="B36" s="18" t="s">
+      <c r="B36" s="23" t="s">
         <v>398</v>
       </c>
       <c r="C36" s="8" t="s">
@@ -10528,31 +10585,31 @@
       </c>
     </row>
     <row r="37" spans="1:4" ht="15" customHeight="1">
-      <c r="A37" s="21"/>
-      <c r="B37" s="18"/>
+      <c r="A37" s="27"/>
+      <c r="B37" s="23"/>
       <c r="C37" s="9" t="s">
         <v>402</v>
       </c>
     </row>
     <row r="38" spans="1:4" ht="15" customHeight="1">
-      <c r="A38" s="20"/>
+      <c r="A38" s="28"/>
     </row>
     <row r="39" spans="1:4" ht="15" customHeight="1">
-      <c r="A39" s="20"/>
-      <c r="C39" s="22"/>
-      <c r="D39" s="23"/>
+      <c r="A39" s="28"/>
+      <c r="C39" s="18"/>
+      <c r="D39" s="19"/>
     </row>
     <row r="40" spans="1:4" ht="15" customHeight="1">
-      <c r="A40" s="20"/>
+      <c r="A40" s="28"/>
     </row>
     <row r="41" spans="1:4" ht="15" customHeight="1">
-      <c r="A41" s="20"/>
+      <c r="A41" s="28"/>
     </row>
     <row r="42" spans="1:4" ht="15" customHeight="1">
-      <c r="A42" s="20"/>
+      <c r="A42" s="28"/>
     </row>
     <row r="43" spans="1:4" ht="15" customHeight="1">
-      <c r="A43" s="20"/>
+      <c r="A43" s="28"/>
     </row>
   </sheetData>
   <mergeCells count="39">
@@ -10564,6 +10621,8 @@
     <mergeCell ref="A30:A31"/>
     <mergeCell ref="A32:A33"/>
     <mergeCell ref="A34:A35"/>
+    <mergeCell ref="B32:B33"/>
+    <mergeCell ref="B34:B35"/>
     <mergeCell ref="B2:B3"/>
     <mergeCell ref="B10:B11"/>
     <mergeCell ref="A36:A37"/>
@@ -10580,8 +10639,6 @@
     <mergeCell ref="A16:A17"/>
     <mergeCell ref="A18:A19"/>
     <mergeCell ref="A20:A21"/>
-    <mergeCell ref="B32:B33"/>
-    <mergeCell ref="B34:B35"/>
     <mergeCell ref="B4:B5"/>
     <mergeCell ref="B28:B29"/>
     <mergeCell ref="B30:B31"/>
@@ -10602,11 +10659,11 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A2:E6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>